<commit_message>
Simulação - 2 estruturas 2 tentativa
Realizou-se a SGSIM (50 realizações) utilizando o modelo variográfico de 2 estrutura. Vale ressaltar que a simulação utilizando o modelo de 2 estrutura só rodou na versão de Práticas do Sgems. Os checks do modelo serão realizados em uma versão mais estável do Sgems, que possa demonstrar de forma clara os histogramas e variogramas simulados.
</commit_message>
<xml_diff>
--- a/SGS/Variogram_1str/SGS.xlsx
+++ b/SGS/Variogram_1str/SGS.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="59">
   <si>
     <t xml:space="preserve">Variável Primária:</t>
   </si>
@@ -160,9 +160,15 @@
     <t xml:space="preserve">Sill</t>
   </si>
   <si>
+    <t xml:space="preserve">4,49+3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Range</t>
   </si>
   <si>
+    <t xml:space="preserve">40+28</t>
+  </si>
+  <si>
     <t xml:space="preserve">n estruturas</t>
   </si>
   <si>
@@ -172,13 +178,28 @@
     <t xml:space="preserve">sph</t>
   </si>
   <si>
+    <t xml:space="preserve">sph+sph</t>
+  </si>
+  <si>
     <t xml:space="preserve">Estrutura 1</t>
   </si>
   <si>
+    <t xml:space="preserve">4.49</t>
+  </si>
+  <si>
     <t xml:space="preserve">Direção</t>
   </si>
   <si>
+    <t xml:space="preserve">Estrutura 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cu_nscore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,5+0,35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44+32</t>
   </si>
 </sst>
 </file>
@@ -193,14 +214,15 @@
     <numFmt numFmtId="168" formatCode="0.00000"/>
     <numFmt numFmtId="169" formatCode="0.000"/>
     <numFmt numFmtId="170" formatCode="0.000000"/>
-    <numFmt numFmtId="171" formatCode="\ * #,##0.00\ ;\-* #,##0.00\ ;\ * \-#\ ;\ @\ "/>
+    <numFmt numFmtId="171" formatCode="* #,##0.00\ ;\-* #,##0.00\ ;* \-#\ ;@\ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -218,87 +240,11 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -307,6 +253,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -314,17 +261,20 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -332,56 +282,15 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFEEEEEE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF666699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -399,6 +308,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB2B2B2"/>
         <bgColor rgb="FFADC5E7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
     <fill>
@@ -426,27 +341,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -471,7 +371,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -497,287 +397,211 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="2" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="15" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="13" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFF2F2F2"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF7DA7D8"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFEEEEEE"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -791,13 +615,13 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFF2F2F2"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FFADC5E7"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1016,21 +840,21 @@
       <c r="D15" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4"/>
+      <c r="A18" s="15"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="16"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="17"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0"/>
@@ -1075,7 +899,8 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1099,7 +924,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="18"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,21 +935,21 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="18"/>
+      <c r="H3" s="19"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
@@ -1134,7 +959,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="18"/>
+      <c r="H5" s="19"/>
       <c r="I5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,88 +970,88 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="18"/>
+      <c r="H6" s="19"/>
       <c r="I6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18"/>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23"/>
-      <c r="B9" s="26" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23"/>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23"/>
-      <c r="B11" s="26" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18"/>
-      <c r="B12" s="26" t="s">
+      <c r="A12" s="19"/>
+      <c r="B12" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1443,6 +1268,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.77"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1457,28 +1283,28 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="V1" s="27" t="s">
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="V1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L2" s="4"/>
@@ -1523,17 +1349,17 @@
       <c r="AD3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -1574,17 +1400,17 @@
       <c r="AD5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -1607,14 +1433,6 @@
       <c r="AD6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -1668,13 +1486,13 @@
       <c r="B9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -1695,16 +1513,16 @@
       <c r="AD9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -1725,16 +1543,16 @@
       <c r="AD10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
@@ -1883,17 +1701,17 @@
       <c r="AD15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -1978,13 +1796,13 @@
       <c r="B19" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
@@ -2006,16 +1824,16 @@
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
@@ -2037,16 +1855,16 @@
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -2142,28 +1960,28 @@
       <c r="G24" s="0"/>
       <c r="H24" s="0"/>
       <c r="I24" s="0"/>
-      <c r="L24" s="27" t="s">
+      <c r="L24" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="27"/>
-      <c r="T24" s="27"/>
-      <c r="V24" s="27" t="s">
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+      <c r="V24" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="W24" s="27"/>
-      <c r="X24" s="27"/>
-      <c r="Y24" s="27"/>
-      <c r="Z24" s="27"/>
-      <c r="AA24" s="27"/>
-      <c r="AB24" s="27"/>
-      <c r="AC24" s="27"/>
-      <c r="AD24" s="27"/>
+      <c r="W24" s="28"/>
+      <c r="X24" s="28"/>
+      <c r="Y24" s="28"/>
+      <c r="Z24" s="28"/>
+      <c r="AA24" s="28"/>
+      <c r="AB24" s="28"/>
+      <c r="AC24" s="28"/>
+      <c r="AD24" s="28"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
@@ -2346,15 +2164,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T44" activeCellId="0" sqref="T44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,6 +2192,19 @@
       </c>
       <c r="H1" s="34"/>
       <c r="I1" s="34"/>
+      <c r="L1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2378,6 +2212,10 @@
         <v>25</v>
       </c>
       <c r="B3" s="35"/>
+      <c r="L3" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="35"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="36" t="s">
@@ -2386,6 +2224,12 @@
       <c r="B4" s="36" t="n">
         <v>20</v>
       </c>
+      <c r="L4" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="36" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="36" t="s">
@@ -2394,6 +2238,12 @@
       <c r="B5" s="36" t="n">
         <v>20</v>
       </c>
+      <c r="L5" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="36" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="36" t="s">
@@ -2402,131 +2252,243 @@
       <c r="B6" s="36" t="n">
         <v>10</v>
       </c>
+      <c r="L6" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="36" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="36" t="n">
         <v>22.5</v>
       </c>
+      <c r="L7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="36" t="n">
+        <v>22.5</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="36" t="n">
         <v>11.25</v>
       </c>
-    </row>
+      <c r="L8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="36" t="n">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="35" t="s">
         <v>42</v>
       </c>
       <c r="B11" s="35"/>
+      <c r="L11" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" s="35"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="37" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="36" t="n">
         <v>3</v>
       </c>
+      <c r="L12" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="36" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="37" t="s">
         <v>44</v>
       </c>
       <c r="B13" s="36" t="n">
         <v>5.99</v>
       </c>
+      <c r="L13" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="M13" s="36" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="38" t="s">
-        <v>45</v>
+      <c r="A14" s="37" t="s">
+        <v>46</v>
       </c>
       <c r="B14" s="36" t="n">
         <v>38</v>
       </c>
+      <c r="L14" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="M14" s="36" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="38" t="s">
-        <v>46</v>
+      <c r="A15" s="37" t="s">
+        <v>48</v>
       </c>
       <c r="B15" s="36" t="n">
         <v>1</v>
       </c>
+      <c r="L15" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" s="36" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="38" t="s">
-        <v>47</v>
+      <c r="A16" s="37" t="s">
+        <v>49</v>
       </c>
       <c r="B16" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="M16" s="36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="36"/>
+      <c r="L19" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="M19" s="36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="40" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="D20" s="40" t="n">
+        <v>45</v>
+      </c>
+      <c r="E20" s="40" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="F20" s="40" t="n">
+        <v>90</v>
+      </c>
+      <c r="G20" s="40" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="H20" s="40" t="n">
+        <v>135</v>
+      </c>
+      <c r="I20" s="40" t="n">
+        <v>157.5</v>
+      </c>
+      <c r="L20" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="M20" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="40" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="O20" s="40" t="n">
+        <v>45</v>
+      </c>
+      <c r="P20" s="40" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="Q20" s="40" t="n">
+        <v>90</v>
+      </c>
+      <c r="R20" s="40" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="S20" s="40" t="n">
+        <v>135</v>
+      </c>
+      <c r="T20" s="40" t="n">
+        <v>157.5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="42" t="n">
+        <v>60</v>
+      </c>
+      <c r="C21" s="42" t="n">
+        <v>42</v>
+      </c>
+      <c r="D21" s="42" t="n">
+        <v>28</v>
+      </c>
+      <c r="E21" s="42" t="n">
+        <v>24</v>
+      </c>
+      <c r="F21" s="42" t="n">
+        <v>28</v>
+      </c>
+      <c r="G21" s="42" t="n">
+        <v>32</v>
+      </c>
+      <c r="H21" s="42" t="n">
+        <v>44</v>
+      </c>
+      <c r="I21" s="42" t="n">
+        <v>62</v>
+      </c>
+      <c r="L21" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="M21" s="42"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="42" t="n">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="36"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="41" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="41" t="n">
-        <v>22.5</v>
-      </c>
-      <c r="D20" s="41" t="n">
-        <v>45</v>
-      </c>
-      <c r="E20" s="41" t="n">
-        <v>67.5</v>
-      </c>
-      <c r="F20" s="41" t="n">
-        <v>90</v>
-      </c>
-      <c r="G20" s="41" t="n">
-        <v>112.5</v>
-      </c>
-      <c r="H20" s="41" t="n">
-        <v>135</v>
-      </c>
-      <c r="I20" s="41" t="n">
-        <v>157.5</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="43" t="n">
-        <v>60</v>
-      </c>
-      <c r="C21" s="43" t="n">
-        <v>42</v>
-      </c>
-      <c r="D21" s="43" t="n">
-        <v>28</v>
-      </c>
-      <c r="E21" s="43" t="n">
-        <v>24</v>
-      </c>
-      <c r="F21" s="43" t="n">
-        <v>28</v>
-      </c>
-      <c r="G21" s="43" t="n">
-        <v>32</v>
-      </c>
-      <c r="H21" s="43" t="n">
-        <v>44</v>
-      </c>
-      <c r="I21" s="43" t="n">
-        <v>62</v>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="42"/>
+      <c r="S21" s="42"/>
+      <c r="T21" s="42" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L22" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="M22" s="36" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2539,20 +2501,60 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="34" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H23" s="34"/>
       <c r="I23" s="34"/>
+      <c r="L23" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="M23" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" s="40" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="O23" s="40" t="n">
+        <v>45</v>
+      </c>
+      <c r="P23" s="40" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="Q23" s="40" t="n">
+        <v>90</v>
+      </c>
+      <c r="R23" s="40" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="S23" s="40" t="n">
+        <v>135</v>
+      </c>
+      <c r="T23" s="40" t="n">
+        <v>157.5</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J24" s="44"/>
+      <c r="L24" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="42"/>
+      <c r="S24" s="42"/>
+      <c r="T24" s="42" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="35" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="35"/>
-      <c r="J25" s="44"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="36" t="s">
@@ -2561,16 +2563,27 @@
       <c r="B26" s="36" t="n">
         <v>20</v>
       </c>
-      <c r="J26" s="44"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="36" t="n">
         <v>20</v>
       </c>
-      <c r="J27" s="44"/>
+      <c r="L27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="S27" s="34"/>
+      <c r="T27" s="34"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="36" t="s">
@@ -2579,149 +2592,316 @@
       <c r="B28" s="36" t="n">
         <v>10</v>
       </c>
-      <c r="J28" s="44"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B29" s="36" t="n">
         <v>22.5</v>
       </c>
-      <c r="J29" s="44"/>
+      <c r="L29" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" s="35"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="36" t="n">
         <v>11.25</v>
       </c>
-      <c r="J30" s="44"/>
+      <c r="L30" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="M30" s="36" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J31" s="44"/>
+      <c r="L31" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="M31" s="36" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J32" s="44"/>
+      <c r="L32" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="M32" s="36" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="35" t="s">
         <v>42</v>
       </c>
       <c r="B33" s="35"/>
-      <c r="J33" s="44"/>
+      <c r="L33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M33" s="36" t="n">
+        <v>22.5</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="37" t="s">
         <v>43</v>
       </c>
       <c r="B34" s="36"/>
-      <c r="J34" s="44"/>
+      <c r="L34" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M34" s="36" t="n">
+        <v>11.25</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="37" t="s">
         <v>44</v>
       </c>
       <c r="B35" s="36"/>
-      <c r="J35" s="44"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="36"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="36"/>
+      <c r="L37" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="M37" s="35"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="L38" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="M38" s="36" t="n">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L39" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="M39" s="36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L40" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="M40" s="36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="36"/>
+      <c r="L41" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="M41" s="36" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="40" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="D42" s="40" t="n">
         <v>45</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="J36" s="44"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="38" t="s">
+      <c r="E42" s="40" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="F42" s="40" t="n">
+        <v>90</v>
+      </c>
+      <c r="G42" s="40" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="H42" s="40" t="n">
+        <v>135</v>
+      </c>
+      <c r="I42" s="40" t="n">
+        <v>157.5</v>
+      </c>
+      <c r="L42" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="M42" s="36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="J37" s="44"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="J38" s="44"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J39" s="44"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J40" s="44"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41" s="36"/>
-      <c r="J41" s="44"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="41" t="n">
+      <c r="B43" s="42"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42" t="n">
+        <v>30</v>
+      </c>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L45" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="M45" s="36" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L46" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="M46" s="40" t="n">
         <v>0</v>
       </c>
-      <c r="C42" s="41" t="n">
+      <c r="N46" s="40" t="n">
         <v>22.5</v>
       </c>
-      <c r="D42" s="41" t="n">
+      <c r="O46" s="40" t="n">
         <v>45</v>
       </c>
-      <c r="E42" s="41" t="n">
+      <c r="P46" s="40" t="n">
         <v>67.5</v>
       </c>
-      <c r="F42" s="41" t="n">
+      <c r="Q46" s="40" t="n">
         <v>90</v>
       </c>
-      <c r="G42" s="41" t="n">
+      <c r="R46" s="40" t="n">
         <v>112.5</v>
       </c>
-      <c r="H42" s="41" t="n">
+      <c r="S46" s="40" t="n">
         <v>135</v>
       </c>
-      <c r="I42" s="41" t="n">
+      <c r="T46" s="40" t="n">
         <v>157.5</v>
       </c>
-      <c r="J42" s="44"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="42" t="s">
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L47" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="M47" s="42"/>
+      <c r="N47" s="42"/>
+      <c r="O47" s="42"/>
+      <c r="P47" s="42" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q47" s="42"/>
+      <c r="R47" s="42"/>
+      <c r="S47" s="42"/>
+      <c r="T47" s="42" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L48" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="M48" s="36" t="n">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L49" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="M49" s="40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" s="40" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="O49" s="40" t="n">
         <v>45</v>
       </c>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43" t="n">
-        <v>30</v>
-      </c>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43" t="n">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="P49" s="40" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="Q49" s="40" t="n">
+        <v>90</v>
+      </c>
+      <c r="R49" s="40" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="S49" s="40" t="n">
+        <v>135</v>
+      </c>
+      <c r="T49" s="40" t="n">
+        <v>157.5</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L50" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="M50" s="42"/>
+      <c r="N50" s="42"/>
+      <c r="O50" s="42"/>
+      <c r="P50" s="42" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q50" s="42"/>
+      <c r="R50" s="42"/>
+      <c r="S50" s="42"/>
+      <c r="T50" s="42" t="n">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="16">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:I1"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="R1:T1"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="L3:M3"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="L11:M11"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="G23:I23"/>
     <mergeCell ref="A25:B25"/>
+    <mergeCell ref="L27:Q27"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="L29:M29"/>
     <mergeCell ref="A33:B33"/>
+    <mergeCell ref="L37:M37"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>